<commit_message>
update api testing report
</commit_message>
<xml_diff>
--- a/docs/apis-testing.xlsx
+++ b/docs/apis-testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FORK OH WEB\openhospital-ui\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29F3247-337F-45D0-B9FF-D3B9F376273E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633463A8-FC81-4FE9-90CD-61CDBFEB3208}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1512" yWindow="1020" windowWidth="19524" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
   <si>
     <t>Methods</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Not availables</t>
   </si>
   <si>
-    <t>/examinations</t>
-  </si>
-  <si>
     <t>Examinations (Triage)</t>
   </si>
   <si>
@@ -145,9 +142,6 @@
   </si>
   <si>
     <t>in therapy form Therapy duration in days, weeks and months are missing in api data model</t>
-  </si>
-  <si>
-    <t>In forms we have category of services, service and booking date, also for each service we want to have two arrays: list of non availables days, and the  list of barely Available days</t>
   </si>
   <si>
     <t>/opds/last/{code}</t>
@@ -278,6 +272,50 @@
   </si>
   <si>
     <t>Since we will have the same model for api integration, I think the response data should be standardized. It is the same for put reponse data type. for delete methods some api return true/false, another void. I think this should also be standardized. For delete method we can rely only on response code, but if we should also rely on response data, I think this should be standardized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suggested apis: get the list of bookings, search bookings by the following criteria: date, patient code, service code, create new booking, modify booking, delete booking </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suggested data model:                                                                                                                      Booking{
+  id: number;
+  bookingDate: Date;
+  service: Service;
+  patient: Patient;
+  status: BoookingStatus;
+}
+enum BoookingStatus {
+  "PENDING",
+  "CONFIRMED",
+  "CANCELLED",
+  "SUCCESS",
+  "FAILED",
+}
+Service{
+  id: number;
+  category: Category;
+  name: number;
+  description: string;
+  cost: number;
+}                                                                                                                                                                                  Category{
+  id: number;
+  name: string;
+  description: string;
+}                                                                                                                                                                               
+ServiceAvailability{
+  year: number;
+  month: number;
+  service: Service;
+  unAvailableDays: number[]; //list of unavailables days for the service
+  barelyAvailableDays number[]; // list of barely availables days for the service
+}
+</t>
+  </si>
+  <si>
+    <t>GET categories, GETservices by category,  GET availabilities by service, month and year.</t>
+  </si>
+  <si>
+    <t>Requests parameters should be also commented</t>
   </si>
 </sst>
 </file>
@@ -750,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -760,13 +798,13 @@
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="45.5546875" customWidth="1"/>
     <col min="4" max="4" width="73.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" width="42.5546875" customWidth="1"/>
     <col min="6" max="6" width="85.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -793,15 +831,15 @@
         <v>4</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>16</v>
@@ -810,13 +848,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -824,11 +862,11 @@
       <c r="B4" s="19"/>
       <c r="C4" s="18"/>
       <c r="D4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -840,7 +878,7 @@
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -852,6 +890,9 @@
       <c r="D6" t="s">
         <v>11</v>
       </c>
+      <c r="F6" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
@@ -907,35 +948,36 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>40</v>
+      <c r="C12" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="C13" s="4"/>
       <c r="D13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -944,10 +986,10 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
         <v>24</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -956,10 +998,10 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -968,10 +1010,10 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -980,10 +1022,10 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -992,10 +1034,10 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1004,39 +1046,39 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
       <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
         <v>32</v>
-      </c>
-      <c r="C20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="13" t="s">
-        <v>33</v>
       </c>
       <c r="B21" t="s">
         <v>13</v>
       </c>
       <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="E21" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1045,10 +1087,10 @@
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1057,10 +1099,10 @@
         <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1069,10 +1111,10 @@
         <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1081,10 +1123,10 @@
         <v>18</v>
       </c>
       <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1093,10 +1135,10 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" t="s">
         <v>42</v>
-      </c>
-      <c r="D26" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1105,10 +1147,10 @@
         <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1117,36 +1159,36 @@
         <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
         <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1155,10 +1197,10 @@
         <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1167,10 +1209,10 @@
         <v>18</v>
       </c>
       <c r="C32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1179,7 +1221,7 @@
         <v>18</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>15</v>
@@ -1191,36 +1233,36 @@
         <v>18</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B36" t="s">
         <v>13</v>
       </c>
       <c r="C36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
laboratory apis test resport
</commit_message>
<xml_diff>
--- a/docs/apis-testing.xlsx
+++ b/docs/apis-testing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FORK OH WEB\openhospital-ui\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\OH WEB\openhospital-ui\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633463A8-FC81-4FE9-90CD-61CDBFEB3208}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B12EC47-B721-4F96-8881-22EC931E3E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1512" yWindow="1020" windowWidth="19524" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="83">
   <si>
     <t>Methods</t>
   </si>
@@ -316,6 +316,83 @@
   </si>
   <si>
     <t>Requests parameters should be also commented</t>
+  </si>
+  <si>
+    <t>laboratory</t>
+  </si>
+  <si>
+    <t>/laboratories</t>
+  </si>
+  <si>
+    <t>/laboratories/byPatientId/{patId}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is given response but: the responses are duplicated. Also the response model should be standardized for both procedures 1 &amp; 2. For each laboratorydto we need List&lt;laborabotoryrowdto&gt; associated to that laboratory. So we are expected something like this: </t>
+  </si>
+  <si>
+    <t>/laboratories/{code}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">It is working for exam procedure 1 but not it is not working for procedure 2, because DTO is not well defined, instead of  "laboratoryRowList": [ "string" ],  we are expected  "laboratoryRowList": [ {code: ..., description: ...., value: ...}, ]. Also the field </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">inOutPatient can be set in the backend before saving the data because it depends on patient admission. If the patient is admitted inOutPatient="I" if not "O". </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Any way we think that the inOutPatient field can be set directly on the backend endpoint instead of UI to avoid unconsistency on data. The LaboratoryRowDTO is missing the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>value: string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field.</t>
+    </r>
+  </si>
+  <si>
+    <t>It is not working. It is returning a 400 error "Laboratory code mismatch", although the {code} is the same as laboratory.code, perhaps the error is not what it should be</t>
+  </si>
+  <si>
+    <t>It is not working, it is returning 400 error, "laboratory not found", although the laboratory is present in fetched data</t>
+  </si>
+  <si>
+    <t>/laboratories/materials</t>
+  </si>
+  <si>
+    <t>It returns an array of  string which represent the material code, We need a way to get the transtated value depending on the current language or should we translate it directly in the frontend?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is working , but not given all the data. Since it is not paginated, we do  not understand why some data are returned and not all. </t>
   </si>
 </sst>
 </file>
@@ -380,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -417,6 +494,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -487,6 +570,144 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>762000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="ZoneTexte 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E5836D6-C511-483F-8CB8-171BE434D86F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5608320" y="15186660"/>
+          <a:ext cx="5006340" cy="1866900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>[  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>{</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>         code:.... , </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>         material:...,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>         ......, </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>         rows: [  //rows or another</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t> name, it is just an example of property name</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>            {code: ..., description: ...., value: ...},</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>        ]  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>    }, </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t> ]</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -786,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -797,18 +1018,18 @@
     <col min="1" max="1" width="19.109375" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="45.5546875" customWidth="1"/>
-    <col min="4" max="4" width="73.109375" customWidth="1"/>
+    <col min="4" max="4" width="76.109375" customWidth="1"/>
     <col min="5" max="5" width="42.5546875" customWidth="1"/>
     <col min="6" max="6" width="85.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
       <c r="E1" s="11"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -838,19 +1059,19 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="20" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F3" t="s">
@@ -858,32 +1079,32 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="18"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="15"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="18"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="15"/>
+      <c r="E5" s="17"/>
       <c r="F5" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="21"/>
       <c r="C6" t="s">
         <v>6</v>
       </c>
@@ -895,8 +1116,8 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
       <c r="C7" t="s">
         <v>8</v>
       </c>
@@ -905,8 +1126,8 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
       <c r="C8" t="s">
         <v>9</v>
       </c>
@@ -915,8 +1136,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
       <c r="C9" t="s">
         <v>10</v>
       </c>
@@ -925,7 +1146,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
+      <c r="A10" s="20"/>
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -937,7 +1158,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
+      <c r="A11" s="20"/>
       <c r="B11" t="s">
         <v>18</v>
       </c>
@@ -966,7 +1187,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="18" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -981,7 +1202,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
+      <c r="A14" s="18"/>
       <c r="B14" t="s">
         <v>18</v>
       </c>
@@ -993,7 +1214,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
+      <c r="A15" s="18"/>
       <c r="B15" t="s">
         <v>18</v>
       </c>
@@ -1005,7 +1226,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
+      <c r="A16" s="18"/>
       <c r="B16" t="s">
         <v>18</v>
       </c>
@@ -1017,7 +1238,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
+      <c r="A17" s="18"/>
       <c r="B17" t="s">
         <v>18</v>
       </c>
@@ -1029,7 +1250,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
+      <c r="A18" s="18"/>
       <c r="B18" t="s">
         <v>18</v>
       </c>
@@ -1041,7 +1262,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
+      <c r="A19" s="18"/>
       <c r="B19" t="s">
         <v>18</v>
       </c>
@@ -1053,7 +1274,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="16"/>
+      <c r="A20" s="18"/>
       <c r="B20" t="s">
         <v>31</v>
       </c>
@@ -1065,7 +1286,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="15" t="s">
         <v>32</v>
       </c>
       <c r="B21" t="s">
@@ -1082,7 +1303,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="13"/>
+      <c r="A22" s="15"/>
       <c r="B22" t="s">
         <v>18</v>
       </c>
@@ -1094,7 +1315,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
+      <c r="A23" s="15"/>
       <c r="B23" t="s">
         <v>18</v>
       </c>
@@ -1106,7 +1327,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
+      <c r="A24" s="15"/>
       <c r="B24" t="s">
         <v>18</v>
       </c>
@@ -1118,7 +1339,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="13"/>
+      <c r="A25" s="15"/>
       <c r="B25" t="s">
         <v>18</v>
       </c>
@@ -1130,7 +1351,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
+      <c r="A26" s="15"/>
       <c r="B26" t="s">
         <v>18</v>
       </c>
@@ -1142,7 +1363,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
+      <c r="A27" s="15"/>
       <c r="B27" t="s">
         <v>18</v>
       </c>
@@ -1154,7 +1375,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
+      <c r="A28" s="15"/>
       <c r="B28" t="s">
         <v>12</v>
       </c>
@@ -1166,7 +1387,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
+      <c r="A29" s="15"/>
       <c r="B29" t="s">
         <v>31</v>
       </c>
@@ -1178,7 +1399,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="15" t="s">
         <v>48</v>
       </c>
       <c r="B30" t="s">
@@ -1192,7 +1413,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
+      <c r="A31" s="15"/>
       <c r="B31" t="s">
         <v>12</v>
       </c>
@@ -1204,7 +1425,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
+      <c r="A32" s="15"/>
       <c r="B32" t="s">
         <v>18</v>
       </c>
@@ -1216,7 +1437,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="13"/>
+      <c r="A33" s="15"/>
       <c r="B33" t="s">
         <v>18</v>
       </c>
@@ -1228,7 +1449,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="13"/>
+      <c r="A34" s="15"/>
       <c r="B34" t="s">
         <v>18</v>
       </c>
@@ -1240,7 +1461,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="13"/>
+      <c r="A35" s="15"/>
       <c r="B35" t="s">
         <v>31</v>
       </c>
@@ -1265,8 +1486,83 @@
         <v>62</v>
       </c>
     </row>
+    <row r="37" spans="1:4" ht="207" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="18"/>
+      <c r="B38" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="18"/>
+      <c r="B39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="18"/>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="18"/>
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="18"/>
+      <c r="B42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A37:A42"/>
     <mergeCell ref="A21:A29"/>
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="A30:A35"/>
@@ -1281,5 +1577,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update billing requirement analysis
</commit_message>
<xml_diff>
--- a/docs/apis-testing.xlsx
+++ b/docs/apis-testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\OH WEB\openhospital-ui\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDCB41F-62D6-487A-A0AD-C571F387DE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890A9CA8-7C3F-454F-B5C7-93F06A3B7F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="113">
   <si>
     <t>Methods</t>
   </si>
@@ -503,10 +503,22 @@
     <t>/pricesothers , /pricelists, /pricelists/prices, /medicalstockward/{ward_code}</t>
   </si>
   <si>
-    <t>User selects Price Entity related to medical, exam, operation, other or custom element with respect to the Price List associated to patient, If the current patient has a reduction plane, we should get the Price Item with the reduced price from Backend before displaying in the BillItems Table, If the patient does'nt have a reduction plane we should display the selected Price Item. (The backend could eventually improve the logic to avoid multiple apis calls by returning each Price Item with reduced price and available quantity in medical case). The new bill can also contain payments. There should be possibility to search Price to add to billItems table using input search . User should also have the possibility to define the quantity and the price of the bill  item. At the moment the affiliate person is missing in the ui and in the api data model. The ward is missing in the ui. We should check the availability of the medical quantity input by user, for that we could fetch the available medical quantity in the selected ward  using /medicalstockward/{ward_code} api. The functionnality to select the billing patient is missing in the ui.</t>
-  </si>
-  <si>
     <t xml:space="preserve">We can search bills by date periods (this api is not avaible), search by patient (api is missing), search bills by billitem (GET /bills/items), search bills by affiliate person  (GET /bills/pending/affiliate), </t>
+  </si>
+  <si>
+    <t>User selects Price Entity related to medical, exam, operation, other or custom element with respect to the Price List associated to patient, If the current patient has a reduction plane, we should get the Price Item with the reduced price from Backend before displaying in the BillItems Table, If the patient does'nt have a reduction plane we should display the selected Price Item. (The backend could eventually improve the logic to avoid multiple apis calls by returning each Price Item with reduced price and reduction rate). The new bill can also contain payments. There should be possibility to search Price to add to billItems table using input search . User should also have the possibility to define the quantity and the price of the bill  item. At the moment the affiliate person is missing in the ui and in the api data model. The ward is missing in the ui. We should check the availability of the medical quantity input by user, for that we could fetch the available medical quantity in the selected ward  using /medicalstockward/{ward_code} api. The functionnality to select the billing patient is missing in the ui, it could be an autocomplete field at the moment.</t>
+  </si>
+  <si>
+    <t>Admission</t>
+  </si>
+  <si>
+    <t>POST and PUT</t>
+  </si>
+  <si>
+    <t>/admissions</t>
+  </si>
+  <si>
+    <t>those methods are not working, we are getting 400 error code for post and 500 error code for put method</t>
   </si>
 </sst>
 </file>
@@ -615,6 +627,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -626,18 +650,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1126,8 +1138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1141,12 +1153,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
       <c r="E1" s="11"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1176,19 +1188,19 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="16" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="21" t="s">
         <v>52</v>
       </c>
       <c r="F3" t="s">
@@ -1196,32 +1208,32 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="20"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="18"/>
+      <c r="E4" s="22"/>
       <c r="F4" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="20"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="18"/>
+      <c r="E5" s="22"/>
       <c r="F5" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
-      <c r="B6" s="21"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
       <c r="C6" t="s">
         <v>6</v>
       </c>
@@ -1233,8 +1245,8 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" s="21"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
       <c r="C7" t="s">
         <v>8</v>
       </c>
@@ -1243,8 +1255,8 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="B8" s="21"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
       <c r="C8" t="s">
         <v>9</v>
       </c>
@@ -1253,8 +1265,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
-      <c r="B9" s="21"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
       <c r="C9" t="s">
         <v>10</v>
       </c>
@@ -1263,7 +1275,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
+      <c r="A10" s="16"/>
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -1275,7 +1287,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
+      <c r="A11" s="16"/>
       <c r="B11" t="s">
         <v>18</v>
       </c>
@@ -1304,7 +1316,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -1319,7 +1331,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
+      <c r="A14" s="19"/>
       <c r="B14" t="s">
         <v>18</v>
       </c>
@@ -1331,7 +1343,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
+      <c r="A15" s="19"/>
       <c r="B15" t="s">
         <v>18</v>
       </c>
@@ -1343,7 +1355,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
+      <c r="A16" s="19"/>
       <c r="B16" t="s">
         <v>18</v>
       </c>
@@ -1355,7 +1367,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
+      <c r="A17" s="19"/>
       <c r="B17" t="s">
         <v>18</v>
       </c>
@@ -1367,7 +1379,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
+      <c r="A18" s="19"/>
       <c r="B18" t="s">
         <v>18</v>
       </c>
@@ -1379,7 +1391,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
+      <c r="A19" s="19"/>
       <c r="B19" t="s">
         <v>18</v>
       </c>
@@ -1391,7 +1403,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
+      <c r="A20" s="19"/>
       <c r="B20" t="s">
         <v>31</v>
       </c>
@@ -1403,7 +1415,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B21" t="s">
@@ -1420,7 +1432,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="16"/>
+      <c r="A22" s="20"/>
       <c r="B22" t="s">
         <v>18</v>
       </c>
@@ -1432,7 +1444,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="16"/>
+      <c r="A23" s="20"/>
       <c r="B23" t="s">
         <v>18</v>
       </c>
@@ -1444,7 +1456,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="16"/>
+      <c r="A24" s="20"/>
       <c r="B24" t="s">
         <v>18</v>
       </c>
@@ -1456,7 +1468,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="16"/>
+      <c r="A25" s="20"/>
       <c r="B25" t="s">
         <v>18</v>
       </c>
@@ -1468,7 +1480,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="16"/>
+      <c r="A26" s="20"/>
       <c r="B26" t="s">
         <v>18</v>
       </c>
@@ -1480,7 +1492,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="16"/>
+      <c r="A27" s="20"/>
       <c r="B27" t="s">
         <v>18</v>
       </c>
@@ -1492,7 +1504,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="16"/>
+      <c r="A28" s="20"/>
       <c r="B28" t="s">
         <v>12</v>
       </c>
@@ -1504,7 +1516,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="16"/>
+      <c r="A29" s="20"/>
       <c r="B29" t="s">
         <v>31</v>
       </c>
@@ -1516,7 +1528,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="20" t="s">
         <v>48</v>
       </c>
       <c r="B30" t="s">
@@ -1530,7 +1542,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="16"/>
+      <c r="A31" s="20"/>
       <c r="B31" t="s">
         <v>12</v>
       </c>
@@ -1542,7 +1554,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="16"/>
+      <c r="A32" s="20"/>
       <c r="B32" t="s">
         <v>18</v>
       </c>
@@ -1554,7 +1566,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="16"/>
+      <c r="A33" s="20"/>
       <c r="B33" t="s">
         <v>18</v>
       </c>
@@ -1566,7 +1578,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="16"/>
+      <c r="A34" s="20"/>
       <c r="B34" t="s">
         <v>18</v>
       </c>
@@ -1578,7 +1590,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="16"/>
+      <c r="A35" s="20"/>
       <c r="B35" t="s">
         <v>31</v>
       </c>
@@ -1604,7 +1616,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="207" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="19" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -1618,7 +1630,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="15"/>
+      <c r="A38" s="19"/>
       <c r="B38" s="13" t="s">
         <v>13</v>
       </c>
@@ -1630,7 +1642,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="15"/>
+      <c r="A39" s="19"/>
       <c r="B39" t="s">
         <v>31</v>
       </c>
@@ -1642,7 +1654,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="15"/>
+      <c r="A40" s="19"/>
       <c r="B40" t="s">
         <v>12</v>
       </c>
@@ -1654,7 +1666,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A41" s="15"/>
+      <c r="A41" s="19"/>
       <c r="B41" t="s">
         <v>18</v>
       </c>
@@ -1666,7 +1678,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="15"/>
+      <c r="A42" s="19"/>
       <c r="B42" t="s">
         <v>18</v>
       </c>
@@ -1705,8 +1717,22 @@
         <v>87</v>
       </c>
     </row>
+    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>109</v>
+      </c>
+      <c r="B45" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" t="s">
+        <v>111</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
     <row r="46" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="18" t="s">
         <v>88</v>
       </c>
       <c r="B46" t="s">
@@ -1716,7 +1742,7 @@
         <v>96</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>106</v>
@@ -1726,7 +1752,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="22"/>
+      <c r="A47" s="18"/>
       <c r="B47" t="s">
         <v>89</v>
       </c>
@@ -1738,7 +1764,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="22"/>
+      <c r="A48" s="18"/>
       <c r="B48" t="s">
         <v>90</v>
       </c>
@@ -1750,7 +1776,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="22"/>
+      <c r="A49" s="18"/>
       <c r="B49" t="s">
         <v>91</v>
       </c>
@@ -1762,7 +1788,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A50" s="22"/>
+      <c r="A50" s="18"/>
       <c r="B50" t="s">
         <v>101</v>
       </c>
@@ -1774,7 +1800,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="22"/>
+      <c r="A51" s="18"/>
       <c r="B51" t="s">
         <v>93</v>
       </c>
@@ -1783,7 +1809,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A52" s="22"/>
+      <c r="A52" s="18"/>
       <c r="B52" t="s">
         <v>92</v>
       </c>
@@ -1791,11 +1817,14 @@
         <v>104</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="A13:A20"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="B3:B9"/>
@@ -1803,9 +1832,6 @@
     <mergeCell ref="A46:A52"/>
     <mergeCell ref="A37:A42"/>
     <mergeCell ref="A21:A29"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="A13:A20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C28" r:id="rId1" location="!/opd-controller/deleteOpdUsingDELETE" display="https://www.open-hospital.org/oh-api/swagger-ui.html - !/opd-controller/deleteOpdUsingDELETE" xr:uid="{21430B8C-249D-4FA6-86BD-8FC9645B744E}"/>

</xml_diff>

<commit_message>
Working edit action on bill item and bill payment tables
</commit_message>
<xml_diff>
--- a/docs/apis-testing.xlsx
+++ b/docs/apis-testing.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\OH WEB\openhospital-ui\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uni2grow\Documents\Open Hospital\openhospital-ui\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DC8AC9-66B9-4172-BB1B-315BED664B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="116">
   <si>
     <t>Methods</t>
   </si>
@@ -520,11 +519,20 @@
   <si>
     <t>those methods are not working, we are getting 400 error code for post and 500 error code for put method</t>
   </si>
+  <si>
+    <t>NEW BILL</t>
+  </si>
+  <si>
+    <t>GET/operations</t>
+  </si>
+  <si>
+    <t>We need operations to fill in the autocomplete when the User chooses Operation Type</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -627,6 +635,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -641,15 +658,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -680,7 +688,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{F353E5D1-8057-4D2E-8CE0-B73C63123379}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1135,30 +1143,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="45.5546875" customWidth="1"/>
-    <col min="4" max="4" width="76.109375" customWidth="1"/>
-    <col min="5" max="5" width="42.5546875" customWidth="1"/>
-    <col min="6" max="6" width="85.33203125" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" customWidth="1"/>
+    <col min="4" max="4" width="76.140625" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" customWidth="1"/>
+    <col min="6" max="6" width="85.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
       <c r="E1" s="11"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1167,7 +1175,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1187,53 +1195,53 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="16" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="21" t="s">
         <v>52</v>
       </c>
       <c r="F3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="21"/>
+    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="19"/>
+      <c r="E4" s="22"/>
       <c r="F4" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="21"/>
+    <row r="5" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="19"/>
+      <c r="E5" s="22"/>
       <c r="F5" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
-      <c r="B6" s="22"/>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
       <c r="C6" t="s">
         <v>6</v>
       </c>
@@ -1244,9 +1252,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="22"/>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
       <c r="C7" t="s">
         <v>8</v>
       </c>
@@ -1254,9 +1262,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
-      <c r="B8" s="22"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
       <c r="C8" t="s">
         <v>9</v>
       </c>
@@ -1264,9 +1272,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
-      <c r="B9" s="22"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
       <c r="C9" t="s">
         <v>10</v>
       </c>
@@ -1274,8 +1282,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -1286,8 +1294,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
       <c r="B11" t="s">
         <v>18</v>
       </c>
@@ -1298,7 +1306,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="409.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>5</v>
       </c>
@@ -1315,8 +1323,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:11" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -1330,8 +1338,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
       <c r="B14" t="s">
         <v>18</v>
       </c>
@@ -1342,8 +1350,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
       <c r="B15" t="s">
         <v>18</v>
       </c>
@@ -1354,8 +1362,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
       <c r="B16" t="s">
         <v>18</v>
       </c>
@@ -1366,8 +1374,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="19"/>
       <c r="B17" t="s">
         <v>18</v>
       </c>
@@ -1378,8 +1386,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
       <c r="B18" t="s">
         <v>18</v>
       </c>
@@ -1390,8 +1398,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
       <c r="B19" t="s">
         <v>18</v>
       </c>
@@ -1402,8 +1410,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="16"/>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
       <c r="B20" t="s">
         <v>31</v>
       </c>
@@ -1414,8 +1422,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
+    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B21" t="s">
@@ -1431,8 +1439,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
       <c r="B22" t="s">
         <v>18</v>
       </c>
@@ -1443,8 +1451,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
       <c r="B23" t="s">
         <v>18</v>
       </c>
@@ -1455,8 +1463,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
       <c r="B24" t="s">
         <v>18</v>
       </c>
@@ -1467,8 +1475,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="20"/>
       <c r="B25" t="s">
         <v>18</v>
       </c>
@@ -1479,8 +1487,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
       <c r="B26" t="s">
         <v>18</v>
       </c>
@@ -1491,8 +1499,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
       <c r="B27" t="s">
         <v>18</v>
       </c>
@@ -1503,8 +1511,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="17"/>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="20"/>
       <c r="B28" t="s">
         <v>12</v>
       </c>
@@ -1515,8 +1523,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="17"/>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
       <c r="B29" t="s">
         <v>31</v>
       </c>
@@ -1527,8 +1535,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="17" t="s">
+    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
         <v>48</v>
       </c>
       <c r="B30" t="s">
@@ -1541,8 +1549,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="20"/>
       <c r="B31" t="s">
         <v>12</v>
       </c>
@@ -1553,8 +1561,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="20"/>
       <c r="B32" t="s">
         <v>18</v>
       </c>
@@ -1565,8 +1573,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="17"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="20"/>
       <c r="B33" t="s">
         <v>18</v>
       </c>
@@ -1577,8 +1585,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="17"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="20"/>
       <c r="B34" t="s">
         <v>18</v>
       </c>
@@ -1589,8 +1597,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="17"/>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="20"/>
       <c r="B35" t="s">
         <v>31</v>
       </c>
@@ -1601,7 +1609,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -1615,8 +1623,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="207" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="16" t="s">
+    <row r="37" spans="1:6" ht="207" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -1629,8 +1637,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="16"/>
+    <row r="38" spans="1:6" ht="105.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="19"/>
       <c r="B38" s="13" t="s">
         <v>13</v>
       </c>
@@ -1641,8 +1649,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="16"/>
+    <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="19"/>
       <c r="B39" t="s">
         <v>31</v>
       </c>
@@ -1653,8 +1661,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="16"/>
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="19"/>
       <c r="B40" t="s">
         <v>12</v>
       </c>
@@ -1665,8 +1673,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A41" s="16"/>
+    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="19"/>
       <c r="B41" t="s">
         <v>18</v>
       </c>
@@ -1677,8 +1685,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="16"/>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="19"/>
       <c r="B42" t="s">
         <v>18</v>
       </c>
@@ -1689,7 +1697,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -1703,7 +1711,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>32</v>
       </c>
@@ -1717,7 +1725,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>109</v>
       </c>
@@ -1731,8 +1739,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A46" s="15" t="s">
+    <row r="46" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+      <c r="A46" s="18" t="s">
         <v>88</v>
       </c>
       <c r="B46" t="s">
@@ -1751,8 +1759,8 @@
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="15"/>
+    <row r="47" spans="1:6" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="18"/>
       <c r="B47" t="s">
         <v>89</v>
       </c>
@@ -1763,8 +1771,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="15"/>
+    <row r="48" spans="1:6" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="18"/>
       <c r="B48" t="s">
         <v>90</v>
       </c>
@@ -1775,8 +1783,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="15"/>
+    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="18"/>
       <c r="B49" t="s">
         <v>91</v>
       </c>
@@ -1787,8 +1795,8 @@
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A50" s="15"/>
+    <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="18"/>
       <c r="B50" t="s">
         <v>101</v>
       </c>
@@ -1799,8 +1807,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="15"/>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="18"/>
       <c r="B51" t="s">
         <v>93</v>
       </c>
@@ -1808,8 +1816,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A52" s="15"/>
+    <row r="52" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="18"/>
       <c r="B52" t="s">
         <v>92</v>
       </c>
@@ -1820,21 +1828,33 @@
         <v>107</v>
       </c>
     </row>
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="18"/>
+      <c r="B53" t="s">
+        <v>113</v>
+      </c>
+      <c r="C53" t="s">
+        <v>114</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="A13:A20"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="B3:B9"/>
     <mergeCell ref="A3:A11"/>
-    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="A46:A53"/>
     <mergeCell ref="A37:A42"/>
     <mergeCell ref="A21:A29"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="A13:A20"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C28" r:id="rId1" location="!/opd-controller/deleteOpdUsingDELETE" display="https://www.open-hospital.org/oh-api/swagger-ui.html - !/opd-controller/deleteOpdUsingDELETE" xr:uid="{21430B8C-249D-4FA6-86BD-8FC9645B744E}"/>
+    <hyperlink ref="C28" r:id="rId1" location="!/opd-controller/deleteOpdUsingDELETE" display="https://www.open-hospital.org/oh-api/swagger-ui.html - !/opd-controller/deleteOpdUsingDELETE"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>

</xml_diff>

<commit_message>
Updated new bill business Logic, fixed payment edit action logic
</commit_message>
<xml_diff>
--- a/docs/apis-testing.xlsx
+++ b/docs/apis-testing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="113">
   <si>
     <t>Methods</t>
   </si>
@@ -499,15 +499,9 @@
     <t>There is no api available to manually close bill, we could use PUT api at the moment</t>
   </si>
   <si>
-    <t>/pricesothers , /pricelists, /pricelists/prices, /medicalstockward/{ward_code}</t>
-  </si>
-  <si>
     <t xml:space="preserve">We can search bills by date periods (this api is not avaible), search by patient (api is missing), search bills by billitem (GET /bills/items), search bills by affiliate person  (GET /bills/pending/affiliate), </t>
   </si>
   <si>
-    <t>User selects Price Entity related to medical, exam, operation, other or custom element with respect to the Price List associated to patient, If the current patient has a reduction plane, we should get the Price Item with the reduced price from Backend before displaying in the BillItems Table, If the patient does'nt have a reduction plane we should display the selected Price Item. (The backend could eventually improve the logic to avoid multiple apis calls by returning each Price Item with reduced price and reduction rate). The new bill can also contain payments. There should be possibility to search Price to add to billItems table using input search . User should also have the possibility to define the quantity and the price of the bill  item. At the moment the affiliate person is missing in the ui and in the api data model. The ward is missing in the ui. We should check the availability of the medical quantity input by user, for that we could fetch the available medical quantity in the selected ward  using /medicalstockward/{ward_code} api. The functionnality to select the billing patient is missing in the ui, it could be an autocomplete field at the moment.</t>
-  </si>
-  <si>
     <t>Admission</t>
   </si>
   <si>
@@ -520,13 +514,10 @@
     <t>those methods are not working, we are getting 400 error code for post and 500 error code for put method</t>
   </si>
   <si>
-    <t>NEW BILL</t>
-  </si>
-  <si>
-    <t>GET/operations</t>
-  </si>
-  <si>
-    <t>We need operations to fill in the autocomplete when the User chooses Operation Type</t>
+    <t>User selects Price Entity related to medical, exam, operation, other or custom element with respect to the Price List associated to patient, If the current patient has a reduction plane, we should get the Price Item with the reduced price from Backend before displaying in the BillItems Table, If the patient does'nt have a reduction plane we should display the selected Price Item. (The backend could eventually improve the logic to avoid multiple apis calls by returning each Price Item with reduced price and reduction rate). The new bill can also contain payments. There should be possibility to search Price to add to billItems table using input search . User should also have the possibility to define the quantity and the price of the bill  item. At the moment the affiliate person is missing in the ui and in the api data model. The ward is missing in the ui. We should check the availability of the medical quantity input by user, for that we could fetch the available medical quantity in the selected ward  using /medicalstockward/{ward_code} api. The functionnality to select the billing patient is missing in the ui, it could be an autocomplete field at the moment. Amount item types, there are operations, therefore we also need to get operations from backend.</t>
+  </si>
+  <si>
+    <t>/pricesothers , /pricelists, /pricelists/prices, /medicalstockward/{ward_code},/operations</t>
   </si>
 </sst>
 </file>
@@ -635,6 +626,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -646,18 +649,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1146,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="D44" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,12 +1152,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
       <c r="E1" s="11"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1196,19 +1187,19 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="20" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="15" t="s">
         <v>52</v>
       </c>
       <c r="F3" t="s">
@@ -1216,32 +1207,32 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="16"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="22"/>
+      <c r="E4" s="16"/>
       <c r="F4" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="16"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="22"/>
+      <c r="E5" s="16"/>
       <c r="F5" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="21"/>
       <c r="C6" t="s">
         <v>6</v>
       </c>
@@ -1253,8 +1244,8 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
       <c r="C7" t="s">
         <v>8</v>
       </c>
@@ -1263,8 +1254,8 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="17"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
       <c r="C8" t="s">
         <v>9</v>
       </c>
@@ -1273,8 +1264,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
       <c r="C9" t="s">
         <v>10</v>
       </c>
@@ -1283,7 +1274,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="A10" s="20"/>
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -1295,7 +1286,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="A11" s="20"/>
       <c r="B11" t="s">
         <v>18</v>
       </c>
@@ -1324,7 +1315,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="18" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -1339,7 +1330,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="18"/>
       <c r="B14" t="s">
         <v>18</v>
       </c>
@@ -1351,7 +1342,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="18"/>
       <c r="B15" t="s">
         <v>18</v>
       </c>
@@ -1363,7 +1354,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="18"/>
       <c r="B16" t="s">
         <v>18</v>
       </c>
@@ -1375,7 +1366,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="18"/>
       <c r="B17" t="s">
         <v>18</v>
       </c>
@@ -1387,7 +1378,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
+      <c r="A18" s="18"/>
       <c r="B18" t="s">
         <v>18</v>
       </c>
@@ -1399,7 +1390,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
+      <c r="A19" s="18"/>
       <c r="B19" t="s">
         <v>18</v>
       </c>
@@ -1411,7 +1402,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="A20" s="18"/>
       <c r="B20" t="s">
         <v>31</v>
       </c>
@@ -1423,7 +1414,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="17" t="s">
         <v>32</v>
       </c>
       <c r="B21" t="s">
@@ -1440,7 +1431,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
+      <c r="A22" s="17"/>
       <c r="B22" t="s">
         <v>18</v>
       </c>
@@ -1452,7 +1443,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
+      <c r="A23" s="17"/>
       <c r="B23" t="s">
         <v>18</v>
       </c>
@@ -1464,7 +1455,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
+      <c r="A24" s="17"/>
       <c r="B24" t="s">
         <v>18</v>
       </c>
@@ -1476,7 +1467,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
+      <c r="A25" s="17"/>
       <c r="B25" t="s">
         <v>18</v>
       </c>
@@ -1488,7 +1479,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
+      <c r="A26" s="17"/>
       <c r="B26" t="s">
         <v>18</v>
       </c>
@@ -1500,7 +1491,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
+      <c r="A27" s="17"/>
       <c r="B27" t="s">
         <v>18</v>
       </c>
@@ -1512,7 +1503,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
+      <c r="A28" s="17"/>
       <c r="B28" t="s">
         <v>12</v>
       </c>
@@ -1524,7 +1515,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
+      <c r="A29" s="17"/>
       <c r="B29" t="s">
         <v>31</v>
       </c>
@@ -1536,7 +1527,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="17" t="s">
         <v>48</v>
       </c>
       <c r="B30" t="s">
@@ -1550,7 +1541,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
+      <c r="A31" s="17"/>
       <c r="B31" t="s">
         <v>12</v>
       </c>
@@ -1562,7 +1553,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
+      <c r="A32" s="17"/>
       <c r="B32" t="s">
         <v>18</v>
       </c>
@@ -1574,7 +1565,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
+      <c r="A33" s="17"/>
       <c r="B33" t="s">
         <v>18</v>
       </c>
@@ -1586,7 +1577,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
+      <c r="A34" s="17"/>
       <c r="B34" t="s">
         <v>18</v>
       </c>
@@ -1598,7 +1589,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
+      <c r="A35" s="17"/>
       <c r="B35" t="s">
         <v>31</v>
       </c>
@@ -1624,7 +1615,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="207" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="18" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -1638,7 +1629,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="105.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="13" t="s">
         <v>13</v>
       </c>
@@ -1650,7 +1641,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
+      <c r="A39" s="18"/>
       <c r="B39" t="s">
         <v>31</v>
       </c>
@@ -1662,7 +1653,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
+      <c r="A40" s="18"/>
       <c r="B40" t="s">
         <v>12</v>
       </c>
@@ -1674,7 +1665,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="19"/>
+      <c r="A41" s="18"/>
       <c r="B41" t="s">
         <v>18</v>
       </c>
@@ -1686,7 +1677,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
+      <c r="A42" s="18"/>
       <c r="B42" t="s">
         <v>18</v>
       </c>
@@ -1727,20 +1718,20 @@
     </row>
     <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>107</v>
+      </c>
+      <c r="B45" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" t="s">
         <v>109</v>
       </c>
-      <c r="B45" t="s">
+      <c r="D45" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C45" t="s">
-        <v>111</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="225" x14ac:dyDescent="0.25">
-      <c r="A46" s="18" t="s">
+    </row>
+    <row r="46" spans="1:6" ht="255" x14ac:dyDescent="0.25">
+      <c r="A46" s="22" t="s">
         <v>88</v>
       </c>
       <c r="B46" t="s">
@@ -1750,17 +1741,17 @@
         <v>96</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="F46" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
+      <c r="A47" s="22"/>
       <c r="B47" t="s">
         <v>89</v>
       </c>
@@ -1772,7 +1763,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="18"/>
+      <c r="A48" s="22"/>
       <c r="B48" t="s">
         <v>90</v>
       </c>
@@ -1784,7 +1775,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
+      <c r="A49" s="22"/>
       <c r="B49" t="s">
         <v>91</v>
       </c>
@@ -1796,7 +1787,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="18"/>
+      <c r="A50" s="22"/>
       <c r="B50" t="s">
         <v>101</v>
       </c>
@@ -1808,7 +1799,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="18"/>
+      <c r="A51" s="22"/>
       <c r="B51" t="s">
         <v>93</v>
       </c>
@@ -1817,7 +1808,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="18"/>
+      <c r="A52" s="22"/>
       <c r="B52" t="s">
         <v>92</v>
       </c>
@@ -1825,23 +1816,18 @@
         <v>104</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="18"/>
-      <c r="B53" t="s">
-        <v>113</v>
-      </c>
-      <c r="C53" t="s">
-        <v>114</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>115</v>
-      </c>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="22"/>
+      <c r="D53" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A46:A53"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="A21:A29"/>
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="A30:A35"/>
     <mergeCell ref="A13:A20"/>
@@ -1849,9 +1835,6 @@
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="B3:B9"/>
     <mergeCell ref="A3:A11"/>
-    <mergeCell ref="A46:A53"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="A21:A29"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C28" r:id="rId1" location="!/opd-controller/deleteOpdUsingDELETE" display="https://www.open-hospital.org/oh-api/swagger-ui.html - !/opd-controller/deleteOpdUsingDELETE"/>

</xml_diff>